<commit_message>
Se le agrega los simbolos para busqueda combinada
</commit_message>
<xml_diff>
--- a/src/combinaciones_palabras.xlsx
+++ b/src/combinaciones_palabras.xlsx
@@ -443,3066 +443,3066 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>genotyping Molecular profiling</t>
+          <t>"genotyping" "Molecular profiling"</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>genotyping Biostatistics</t>
+          <t>"genotyping" "Biostatistics"</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>genotyping Computational biology</t>
+          <t>"genotyping" "Computational biology"</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>genotyping microbial ecology</t>
+          <t>"genotyping" "microbial ecology"</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>genotyping Microbial interactions</t>
+          <t>"genotyping" "Microbial interactions"</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>genotyping Water supply</t>
+          <t>"genotyping" "Water supply"</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>genotyping climate change</t>
+          <t>"genotyping" "climate change"</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Molecular profiling Biostatistics</t>
+          <t>"Molecular profiling" "Biostatistics"</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Molecular profiling Computational biology</t>
+          <t>"Molecular profiling" "Computational biology"</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Molecular profiling microbial ecology</t>
+          <t>"Molecular profiling" "microbial ecology"</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Molecular profiling Microbial interactions</t>
+          <t>"Molecular profiling" "Microbial interactions"</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Molecular profiling Water supply</t>
+          <t>"Molecular profiling" "Water supply"</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Molecular profiling climate change</t>
+          <t>"Molecular profiling" "climate change"</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Biostatistics Computational biology</t>
+          <t>"Biostatistics" "Computational biology"</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Biostatistics microbial ecology</t>
+          <t>"Biostatistics" "microbial ecology"</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Biostatistics Microbial interactions</t>
+          <t>"Biostatistics" "Microbial interactions"</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Biostatistics Water supply</t>
+          <t>"Biostatistics" "Water supply"</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Biostatistics climate change</t>
+          <t>"Biostatistics" "climate change"</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Computational biology microbial ecology</t>
+          <t>"Computational biology" "microbial ecology"</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Computational biology Microbial interactions</t>
+          <t>"Computational biology" "Microbial interactions"</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Computational biology Water supply</t>
+          <t>"Computational biology" "Water supply"</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Computational biology climate change</t>
+          <t>"Computational biology" "climate change"</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>microbial ecology Microbial interactions</t>
+          <t>"microbial ecology" "Microbial interactions"</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>microbial ecology Water supply</t>
+          <t>"microbial ecology" "Water supply"</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>microbial ecology climate change</t>
+          <t>"microbial ecology" "climate change"</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Microbial interactions Water supply</t>
+          <t>"Microbial interactions" "Water supply"</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Microbial interactions climate change</t>
+          <t>"Microbial interactions" "climate change"</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Water supply climate change</t>
+          <t>"Water supply" "climate change"</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>pharmacology Pharmacodynamics</t>
+          <t>"pharmacology" "Pharmacodynamics"</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>pharmacology real world evidence</t>
+          <t>"pharmacology" "real world evidence"</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>pharmacology Substantial evidence</t>
+          <t>"pharmacology" "Substantial evidence"</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>pharmacology chronic diseases</t>
+          <t>"pharmacology" "chronic diseases"</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>pharmacology Chronic illnesses</t>
+          <t>"pharmacology" "Chronic illnesses"</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>pharmacology Chronic conditions</t>
+          <t>"pharmacology" "Chronic conditions"</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>pharmacology Chronic health conditions</t>
+          <t>"pharmacology" "Chronic health conditions"</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>pharmacology Chronic kidney disease</t>
+          <t>"pharmacology" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>pharmacology COPD</t>
+          <t>"pharmacology" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>pharmacology Health management</t>
+          <t>"pharmacology" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>pharmacology Health administration</t>
+          <t>"pharmacology" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Pharmacodynamics real world evidence</t>
+          <t>"Pharmacodynamics" "real world evidence"</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Pharmacodynamics Substantial evidence</t>
+          <t>"Pharmacodynamics" "Substantial evidence"</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Pharmacodynamics chronic diseases</t>
+          <t>"Pharmacodynamics" "chronic diseases"</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Pharmacodynamics Chronic illnesses</t>
+          <t>"Pharmacodynamics" "Chronic illnesses"</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Pharmacodynamics Chronic conditions</t>
+          <t>"Pharmacodynamics" "Chronic conditions"</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Pharmacodynamics Chronic health conditions</t>
+          <t>"Pharmacodynamics" "Chronic health conditions"</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Pharmacodynamics Chronic kidney disease</t>
+          <t>"Pharmacodynamics" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Pharmacodynamics COPD</t>
+          <t>"Pharmacodynamics" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Pharmacodynamics Health management</t>
+          <t>"Pharmacodynamics" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Pharmacodynamics Health administration</t>
+          <t>"Pharmacodynamics" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>real world evidence Substantial evidence</t>
+          <t>"real world evidence" "Substantial evidence"</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>real world evidence chronic diseases</t>
+          <t>"real world evidence" "chronic diseases"</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>real world evidence Chronic illnesses</t>
+          <t>"real world evidence" "Chronic illnesses"</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>real world evidence Chronic conditions</t>
+          <t>"real world evidence" "Chronic conditions"</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>real world evidence Chronic health conditions</t>
+          <t>"real world evidence" "Chronic health conditions"</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>real world evidence Chronic kidney disease</t>
+          <t>"real world evidence" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>real world evidence COPD</t>
+          <t>"real world evidence" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>real world evidence Health management</t>
+          <t>"real world evidence" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>real world evidence Health administration</t>
+          <t>"real world evidence" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Substantial evidence chronic diseases</t>
+          <t>"Substantial evidence" "chronic diseases"</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Substantial evidence Chronic illnesses</t>
+          <t>"Substantial evidence" "Chronic illnesses"</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Substantial evidence Chronic conditions</t>
+          <t>"Substantial evidence" "Chronic conditions"</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Substantial evidence Chronic health conditions</t>
+          <t>"Substantial evidence" "Chronic health conditions"</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Substantial evidence Chronic kidney disease</t>
+          <t>"Substantial evidence" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Substantial evidence COPD</t>
+          <t>"Substantial evidence" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Substantial evidence Health management</t>
+          <t>"Substantial evidence" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Substantial evidence Health administration</t>
+          <t>"Substantial evidence" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>chronic diseases Chronic illnesses</t>
+          <t>"chronic diseases" "Chronic illnesses"</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>chronic diseases Chronic conditions</t>
+          <t>"chronic diseases" "Chronic conditions"</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>chronic diseases Chronic health conditions</t>
+          <t>"chronic diseases" "Chronic health conditions"</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>chronic diseases Chronic kidney disease</t>
+          <t>"chronic diseases" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>chronic diseases COPD</t>
+          <t>"chronic diseases" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>chronic diseases Health management</t>
+          <t>"chronic diseases" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>chronic diseases Health administration</t>
+          <t>"chronic diseases" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Chronic illnesses Chronic conditions</t>
+          <t>"Chronic illnesses" "Chronic conditions"</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Chronic illnesses Chronic health conditions</t>
+          <t>"Chronic illnesses" "Chronic health conditions"</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Chronic illnesses Chronic kidney disease</t>
+          <t>"Chronic illnesses" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Chronic illnesses COPD</t>
+          <t>"Chronic illnesses" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Chronic illnesses Health management</t>
+          <t>"Chronic illnesses" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Chronic illnesses Health administration</t>
+          <t>"Chronic illnesses" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Chronic conditions Chronic health conditions</t>
+          <t>"Chronic conditions" "Chronic health conditions"</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Chronic conditions Chronic kidney disease</t>
+          <t>"Chronic conditions" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Chronic conditions COPD</t>
+          <t>"Chronic conditions" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Chronic conditions Health management</t>
+          <t>"Chronic conditions" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Chronic conditions Health administration</t>
+          <t>"Chronic conditions" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Chronic health conditions Chronic kidney disease</t>
+          <t>"Chronic health conditions" "Chronic kidney disease"</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Chronic health conditions COPD</t>
+          <t>"Chronic health conditions" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Chronic health conditions Health management</t>
+          <t>"Chronic health conditions" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Chronic health conditions Health administration</t>
+          <t>"Chronic health conditions" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Chronic kidney disease COPD</t>
+          <t>"Chronic kidney disease" "COPD"</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Chronic kidney disease Health management</t>
+          <t>"Chronic kidney disease" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Chronic kidney disease Health administration</t>
+          <t>"Chronic kidney disease" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>COPD Health management</t>
+          <t>"COPD" "Health management"</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>COPD Health administration</t>
+          <t>"COPD" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Health management Health administration</t>
+          <t>"Health management" "Health administration"</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Clinical research clinical trials </t>
+          <t>"Clinical research" "clinical trials "</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Clinical research Clinical investigations</t>
+          <t>"Clinical research" "Clinical investigations"</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Clinical research Respiratory infection</t>
+          <t>"Clinical research" "Respiratory infection"</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Clinical research Pneumonia</t>
+          <t>"Clinical research" "Pneumonia"</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Clinical research infectious diseases</t>
+          <t>"Clinical research" "infectious diseases"</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Clinical research Communicable diseases</t>
+          <t>"Clinical research" "Communicable diseases"</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Clinical research global health</t>
+          <t>"Clinical research" "global health"</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Clinical research International health</t>
+          <t>"Clinical research" "International health"</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t xml:space="preserve">Clinical research one health </t>
+          <t>"Clinical research" "one health "</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>clinical trials  Clinical investigations</t>
+          <t>"clinical trials " "Clinical investigations"</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>clinical trials  Respiratory infection</t>
+          <t>"clinical trials " "Respiratory infection"</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>clinical trials  Pneumonia</t>
+          <t>"clinical trials " "Pneumonia"</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>clinical trials  infectious diseases</t>
+          <t>"clinical trials " "infectious diseases"</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>clinical trials  Communicable diseases</t>
+          <t>"clinical trials " "Communicable diseases"</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>clinical trials  global health</t>
+          <t>"clinical trials " "global health"</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>clinical trials  International health</t>
+          <t>"clinical trials " "International health"</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t xml:space="preserve">clinical trials  one health </t>
+          <t>"clinical trials " "one health "</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Clinical investigations Respiratory infection</t>
+          <t>"Clinical investigations" "Respiratory infection"</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Clinical investigations Pneumonia</t>
+          <t>"Clinical investigations" "Pneumonia"</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Clinical investigations infectious diseases</t>
+          <t>"Clinical investigations" "infectious diseases"</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Clinical investigations Communicable diseases</t>
+          <t>"Clinical investigations" "Communicable diseases"</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Clinical investigations global health</t>
+          <t>"Clinical investigations" "global health"</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Clinical investigations International health</t>
+          <t>"Clinical investigations" "International health"</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t xml:space="preserve">Clinical investigations one health </t>
+          <t>"Clinical investigations" "one health "</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Respiratory infection Pneumonia</t>
+          <t>"Respiratory infection" "Pneumonia"</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Respiratory infection infectious diseases</t>
+          <t>"Respiratory infection" "infectious diseases"</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Respiratory infection Communicable diseases</t>
+          <t>"Respiratory infection" "Communicable diseases"</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Respiratory infection global health</t>
+          <t>"Respiratory infection" "global health"</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Respiratory infection International health</t>
+          <t>"Respiratory infection" "International health"</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t xml:space="preserve">Respiratory infection one health </t>
+          <t>"Respiratory infection" "one health "</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Pneumonia infectious diseases</t>
+          <t>"Pneumonia" "infectious diseases"</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Pneumonia Communicable diseases</t>
+          <t>"Pneumonia" "Communicable diseases"</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Pneumonia global health</t>
+          <t>"Pneumonia" "global health"</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Pneumonia International health</t>
+          <t>"Pneumonia" "International health"</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pneumonia one health </t>
+          <t>"Pneumonia" "one health "</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>infectious diseases Communicable diseases</t>
+          <t>"infectious diseases" "Communicable diseases"</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>infectious diseases global health</t>
+          <t>"infectious diseases" "global health"</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>infectious diseases International health</t>
+          <t>"infectious diseases" "International health"</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t xml:space="preserve">infectious diseases one health </t>
+          <t>"infectious diseases" "one health "</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Communicable diseases global health</t>
+          <t>"Communicable diseases" "global health"</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Communicable diseases International health</t>
+          <t>"Communicable diseases" "International health"</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t xml:space="preserve">Communicable diseases one health </t>
+          <t>"Communicable diseases" "one health "</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>global health International health</t>
+          <t>"global health" "International health"</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t xml:space="preserve">global health one health </t>
+          <t>"global health" "one health "</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t xml:space="preserve">International health one health </t>
+          <t>"International health" "one health "</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Food insecurity Hunger</t>
+          <t>"Food insecurity" "Hunger"</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Food insecurity Nutrition</t>
+          <t>"Food insecurity" "Nutrition"</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Food insecurity Mathematical modeling</t>
+          <t>"Food insecurity" "Mathematical modeling"</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Food insecurity Analytical modeling</t>
+          <t>"Food insecurity" "Analytical modeling"</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Hunger Nutrition</t>
+          <t>"Hunger" "Nutrition"</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Hunger Mathematical modeling</t>
+          <t>"Hunger" "Mathematical modeling"</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Hunger Analytical modeling</t>
+          <t>"Hunger" "Analytical modeling"</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Nutrition Mathematical modeling</t>
+          <t>"Nutrition" "Mathematical modeling"</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Nutrition Analytical modeling</t>
+          <t>"Nutrition" "Analytical modeling"</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Mathematical modeling Analytical modeling</t>
+          <t>"Mathematical modeling" "Analytical modeling"</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Distress Perturbation</t>
+          <t>"Distress" "Perturbation"</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Distress Sadness</t>
+          <t>"Distress" "Sadness"</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Distress Psychological distress</t>
+          <t>"Distress" "Psychological distress"</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Distress Mental health condition</t>
+          <t>"Distress" "Mental health condition"</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Distress Social networks</t>
+          <t>"Distress" "Social networks"</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Distress health communication</t>
+          <t>"Distress" "health communication"</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Perturbation Sadness</t>
+          <t>"Perturbation" "Sadness"</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Perturbation Psychological distress</t>
+          <t>"Perturbation" "Psychological distress"</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Perturbation Mental health condition</t>
+          <t>"Perturbation" "Mental health condition"</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Perturbation Social networks</t>
+          <t>"Perturbation" "Social networks"</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Perturbation health communication</t>
+          <t>"Perturbation" "health communication"</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Sadness Psychological distress</t>
+          <t>"Sadness" "Psychological distress"</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Sadness Mental health condition</t>
+          <t>"Sadness" "Mental health condition"</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Sadness Social networks</t>
+          <t>"Sadness" "Social networks"</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Sadness health communication</t>
+          <t>"Sadness" "health communication"</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Psychological distress Mental health condition</t>
+          <t>"Psychological distress" "Mental health condition"</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Psychological distress Social networks</t>
+          <t>"Psychological distress" "Social networks"</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Psychological distress health communication</t>
+          <t>"Psychological distress" "health communication"</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Mental health condition Social networks</t>
+          <t>"Mental health condition" "Social networks"</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Mental health condition health communication</t>
+          <t>"Mental health condition" "health communication"</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Social networks health communication</t>
+          <t>"Social networks" "health communication"</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Nanotechnology Nanoscience</t>
+          <t>"Nanotechnology" "Nanoscience"</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Nanotechnology Probiotic strains</t>
+          <t>"Nanotechnology" "Probiotic strains"</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanotechnology microbiota </t>
+          <t>"Nanotechnology" "microbiota "</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanotechnology food safety </t>
+          <t>"Nanotechnology" "food safety "</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Nanotechnology Food Security</t>
+          <t>"Nanotechnology" "Food Security"</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Nanoscience Probiotic strains</t>
+          <t>"Nanoscience" "Probiotic strains"</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanoscience microbiota </t>
+          <t>"Nanoscience" "microbiota "</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nanoscience food safety </t>
+          <t>"Nanoscience" "food safety "</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Nanoscience Food Security</t>
+          <t>"Nanoscience" "Food Security"</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probiotic strains microbiota </t>
+          <t>"Probiotic strains" "microbiota "</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t xml:space="preserve">Probiotic strains food safety </t>
+          <t>"Probiotic strains" "food safety "</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Probiotic strains Food Security</t>
+          <t>"Probiotic strains" "Food Security"</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t xml:space="preserve">microbiota  food safety </t>
+          <t>"microbiota " "food safety "</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>microbiota  Food Security</t>
+          <t>"microbiota " "Food Security"</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>food safety  Food Security</t>
+          <t>"food safety " "Food Security"</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>neuromodulation  Nerve Stimulation</t>
+          <t>"neuromodulation " "Nerve Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>neuromodulation  Neurostimulation</t>
+          <t>"neuromodulation " "Neurostimulation"</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>neuromodulation  Brain Stimulation</t>
+          <t>"neuromodulation " "Brain Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>neuromodulation  Electrical Stimulation</t>
+          <t>"neuromodulation " "Electrical Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>neuromodulation  Neurotechnology</t>
+          <t>"neuromodulation " "Neurotechnology"</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>neuromodulation  Knowledge transfer</t>
+          <t>"neuromodulation " "Knowledge transfer"</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>neuromodulation  Information exchange</t>
+          <t>"neuromodulation " "Information exchange"</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>neuromodulation  Data transmission</t>
+          <t>"neuromodulation " "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>neuromodulation  Traumatic Brain Injury</t>
+          <t>"neuromodulation " "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>neuromodulation  Brain Trauma</t>
+          <t>"neuromodulation " "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuromodulation  neuroinflammation </t>
+          <t>"neuromodulation " "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuromodulation  traumatic brain injury </t>
+          <t>"neuromodulation " "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>neuromodulation  Brain Damage</t>
+          <t>"neuromodulation " "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuromodulation  rehabilitation </t>
+          <t>"neuromodulation " "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>neuromodulation  Rehab</t>
+          <t>"neuromodulation " "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>neuromodulation  Therapy</t>
+          <t>"neuromodulation " "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>neuromodulation  Restoration</t>
+          <t>"neuromodulation " "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>neuromodulation  Recovery Program</t>
+          <t>"neuromodulation " "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuromodulation  Intensive care </t>
+          <t>"neuromodulation " "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>neuromodulation  Critical Care</t>
+          <t>"neuromodulation " "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>neuromodulation  Acute Care</t>
+          <t>"neuromodulation " "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>neuromodulation  Emergency Care</t>
+          <t>"neuromodulation " "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Neurostimulation</t>
+          <t>"Nerve Stimulation" "Neurostimulation"</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Brain Stimulation</t>
+          <t>"Nerve Stimulation" "Brain Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Electrical Stimulation</t>
+          <t>"Nerve Stimulation" "Electrical Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Neurotechnology</t>
+          <t>"Nerve Stimulation" "Neurotechnology"</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Knowledge transfer</t>
+          <t>"Nerve Stimulation" "Knowledge transfer"</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Information exchange</t>
+          <t>"Nerve Stimulation" "Information exchange"</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Data transmission</t>
+          <t>"Nerve Stimulation" "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Traumatic Brain Injury</t>
+          <t>"Nerve Stimulation" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Brain Trauma</t>
+          <t>"Nerve Stimulation" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nerve Stimulation neuroinflammation </t>
+          <t>"Nerve Stimulation" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nerve Stimulation traumatic brain injury </t>
+          <t>"Nerve Stimulation" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Brain Damage</t>
+          <t>"Nerve Stimulation" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nerve Stimulation rehabilitation </t>
+          <t>"Nerve Stimulation" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Rehab</t>
+          <t>"Nerve Stimulation" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Therapy</t>
+          <t>"Nerve Stimulation" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Restoration</t>
+          <t>"Nerve Stimulation" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Recovery Program</t>
+          <t>"Nerve Stimulation" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nerve Stimulation Intensive care </t>
+          <t>"Nerve Stimulation" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Critical Care</t>
+          <t>"Nerve Stimulation" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Acute Care</t>
+          <t>"Nerve Stimulation" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Nerve Stimulation Emergency Care</t>
+          <t>"Nerve Stimulation" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Neurostimulation Brain Stimulation</t>
+          <t>"Neurostimulation" "Brain Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Neurostimulation Electrical Stimulation</t>
+          <t>"Neurostimulation" "Electrical Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Neurostimulation Neurotechnology</t>
+          <t>"Neurostimulation" "Neurotechnology"</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Neurostimulation Knowledge transfer</t>
+          <t>"Neurostimulation" "Knowledge transfer"</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Neurostimulation Information exchange</t>
+          <t>"Neurostimulation" "Information exchange"</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Neurostimulation Data transmission</t>
+          <t>"Neurostimulation" "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Neurostimulation Traumatic Brain Injury</t>
+          <t>"Neurostimulation" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Neurostimulation Brain Trauma</t>
+          <t>"Neurostimulation" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurostimulation neuroinflammation </t>
+          <t>"Neurostimulation" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurostimulation traumatic brain injury </t>
+          <t>"Neurostimulation" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Neurostimulation Brain Damage</t>
+          <t>"Neurostimulation" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurostimulation rehabilitation </t>
+          <t>"Neurostimulation" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Neurostimulation Rehab</t>
+          <t>"Neurostimulation" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Neurostimulation Therapy</t>
+          <t>"Neurostimulation" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Neurostimulation Restoration</t>
+          <t>"Neurostimulation" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Neurostimulation Recovery Program</t>
+          <t>"Neurostimulation" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurostimulation Intensive care </t>
+          <t>"Neurostimulation" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Neurostimulation Critical Care</t>
+          <t>"Neurostimulation" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Neurostimulation Acute Care</t>
+          <t>"Neurostimulation" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Neurostimulation Emergency Care</t>
+          <t>"Neurostimulation" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Brain Stimulation Electrical Stimulation</t>
+          <t>"Brain Stimulation" "Electrical Stimulation"</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Brain Stimulation Neurotechnology</t>
+          <t>"Brain Stimulation" "Neurotechnology"</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Brain Stimulation Knowledge transfer</t>
+          <t>"Brain Stimulation" "Knowledge transfer"</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Brain Stimulation Information exchange</t>
+          <t>"Brain Stimulation" "Information exchange"</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Brain Stimulation Data transmission</t>
+          <t>"Brain Stimulation" "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Brain Stimulation Traumatic Brain Injury</t>
+          <t>"Brain Stimulation" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Brain Stimulation Brain Trauma</t>
+          <t>"Brain Stimulation" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Stimulation neuroinflammation </t>
+          <t>"Brain Stimulation" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Stimulation traumatic brain injury </t>
+          <t>"Brain Stimulation" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Brain Stimulation Brain Damage</t>
+          <t>"Brain Stimulation" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Stimulation rehabilitation </t>
+          <t>"Brain Stimulation" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Brain Stimulation Rehab</t>
+          <t>"Brain Stimulation" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Brain Stimulation Therapy</t>
+          <t>"Brain Stimulation" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Brain Stimulation Restoration</t>
+          <t>"Brain Stimulation" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Brain Stimulation Recovery Program</t>
+          <t>"Brain Stimulation" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Stimulation Intensive care </t>
+          <t>"Brain Stimulation" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Brain Stimulation Critical Care</t>
+          <t>"Brain Stimulation" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Brain Stimulation Acute Care</t>
+          <t>"Brain Stimulation" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Brain Stimulation Emergency Care</t>
+          <t>"Brain Stimulation" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Neurotechnology</t>
+          <t>"Electrical Stimulation" "Neurotechnology"</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Knowledge transfer</t>
+          <t>"Electrical Stimulation" "Knowledge transfer"</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Information exchange</t>
+          <t>"Electrical Stimulation" "Information exchange"</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Data transmission</t>
+          <t>"Electrical Stimulation" "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Traumatic Brain Injury</t>
+          <t>"Electrical Stimulation" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Brain Trauma</t>
+          <t>"Electrical Stimulation" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t xml:space="preserve">Electrical Stimulation neuroinflammation </t>
+          <t>"Electrical Stimulation" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t xml:space="preserve">Electrical Stimulation traumatic brain injury </t>
+          <t>"Electrical Stimulation" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Brain Damage</t>
+          <t>"Electrical Stimulation" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t xml:space="preserve">Electrical Stimulation rehabilitation </t>
+          <t>"Electrical Stimulation" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Rehab</t>
+          <t>"Electrical Stimulation" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Therapy</t>
+          <t>"Electrical Stimulation" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Restoration</t>
+          <t>"Electrical Stimulation" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Recovery Program</t>
+          <t>"Electrical Stimulation" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t xml:space="preserve">Electrical Stimulation Intensive care </t>
+          <t>"Electrical Stimulation" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Critical Care</t>
+          <t>"Electrical Stimulation" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Acute Care</t>
+          <t>"Electrical Stimulation" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Electrical Stimulation Emergency Care</t>
+          <t>"Electrical Stimulation" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Neurotechnology Knowledge transfer</t>
+          <t>"Neurotechnology" "Knowledge transfer"</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Neurotechnology Information exchange</t>
+          <t>"Neurotechnology" "Information exchange"</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Neurotechnology Data transmission</t>
+          <t>"Neurotechnology" "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Neurotechnology Traumatic Brain Injury</t>
+          <t>"Neurotechnology" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Neurotechnology Brain Trauma</t>
+          <t>"Neurotechnology" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurotechnology neuroinflammation </t>
+          <t>"Neurotechnology" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurotechnology traumatic brain injury </t>
+          <t>"Neurotechnology" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Neurotechnology Brain Damage</t>
+          <t>"Neurotechnology" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurotechnology rehabilitation </t>
+          <t>"Neurotechnology" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Neurotechnology Rehab</t>
+          <t>"Neurotechnology" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Neurotechnology Therapy</t>
+          <t>"Neurotechnology" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Neurotechnology Restoration</t>
+          <t>"Neurotechnology" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Neurotechnology Recovery Program</t>
+          <t>"Neurotechnology" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neurotechnology Intensive care </t>
+          <t>"Neurotechnology" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Neurotechnology Critical Care</t>
+          <t>"Neurotechnology" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Neurotechnology Acute Care</t>
+          <t>"Neurotechnology" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Neurotechnology Emergency Care</t>
+          <t>"Neurotechnology" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Knowledge transfer Information exchange</t>
+          <t>"Knowledge transfer" "Information exchange"</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Knowledge transfer Data transmission</t>
+          <t>"Knowledge transfer" "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Knowledge transfer Traumatic Brain Injury</t>
+          <t>"Knowledge transfer" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Knowledge transfer Brain Trauma</t>
+          <t>"Knowledge transfer" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t xml:space="preserve">Knowledge transfer neuroinflammation </t>
+          <t>"Knowledge transfer" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t xml:space="preserve">Knowledge transfer traumatic brain injury </t>
+          <t>"Knowledge transfer" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Knowledge transfer Brain Damage</t>
+          <t>"Knowledge transfer" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t xml:space="preserve">Knowledge transfer rehabilitation </t>
+          <t>"Knowledge transfer" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Knowledge transfer Rehab</t>
+          <t>"Knowledge transfer" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Knowledge transfer Therapy</t>
+          <t>"Knowledge transfer" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Knowledge transfer Restoration</t>
+          <t>"Knowledge transfer" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Knowledge transfer Recovery Program</t>
+          <t>"Knowledge transfer" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t xml:space="preserve">Knowledge transfer Intensive care </t>
+          <t>"Knowledge transfer" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Knowledge transfer Critical Care</t>
+          <t>"Knowledge transfer" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Knowledge transfer Acute Care</t>
+          <t>"Knowledge transfer" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Knowledge transfer Emergency Care</t>
+          <t>"Knowledge transfer" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Information exchange Data transmission</t>
+          <t>"Information exchange" "Data transmission"</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Information exchange Traumatic Brain Injury</t>
+          <t>"Information exchange" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Information exchange Brain Trauma</t>
+          <t>"Information exchange" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information exchange neuroinflammation </t>
+          <t>"Information exchange" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information exchange traumatic brain injury </t>
+          <t>"Information exchange" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>Information exchange Brain Damage</t>
+          <t>"Information exchange" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information exchange rehabilitation </t>
+          <t>"Information exchange" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>Information exchange Rehab</t>
+          <t>"Information exchange" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>Information exchange Therapy</t>
+          <t>"Information exchange" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Information exchange Restoration</t>
+          <t>"Information exchange" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>Information exchange Recovery Program</t>
+          <t>"Information exchange" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t xml:space="preserve">Information exchange Intensive care </t>
+          <t>"Information exchange" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>Information exchange Critical Care</t>
+          <t>"Information exchange" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Information exchange Acute Care</t>
+          <t>"Information exchange" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Information exchange Emergency Care</t>
+          <t>"Information exchange" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Data transmission Traumatic Brain Injury</t>
+          <t>"Data transmission" "Traumatic Brain Injury"</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Data transmission Brain Trauma</t>
+          <t>"Data transmission" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data transmission neuroinflammation </t>
+          <t>"Data transmission" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data transmission traumatic brain injury </t>
+          <t>"Data transmission" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Data transmission Brain Damage</t>
+          <t>"Data transmission" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data transmission rehabilitation </t>
+          <t>"Data transmission" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Data transmission Rehab</t>
+          <t>"Data transmission" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Data transmission Therapy</t>
+          <t>"Data transmission" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Data transmission Restoration</t>
+          <t>"Data transmission" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Data transmission Recovery Program</t>
+          <t>"Data transmission" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t xml:space="preserve">Data transmission Intensive care </t>
+          <t>"Data transmission" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Data transmission Critical Care</t>
+          <t>"Data transmission" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Data transmission Acute Care</t>
+          <t>"Data transmission" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Data transmission Emergency Care</t>
+          <t>"Data transmission" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Brain Trauma</t>
+          <t>"Traumatic Brain Injury" "Brain Trauma"</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traumatic Brain Injury neuroinflammation </t>
+          <t>"Traumatic Brain Injury" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traumatic Brain Injury traumatic brain injury </t>
+          <t>"Traumatic Brain Injury" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Brain Damage</t>
+          <t>"Traumatic Brain Injury" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traumatic Brain Injury rehabilitation </t>
+          <t>"Traumatic Brain Injury" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Rehab</t>
+          <t>"Traumatic Brain Injury" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Therapy</t>
+          <t>"Traumatic Brain Injury" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Restoration</t>
+          <t>"Traumatic Brain Injury" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Recovery Program</t>
+          <t>"Traumatic Brain Injury" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traumatic Brain Injury Intensive care </t>
+          <t>"Traumatic Brain Injury" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Critical Care</t>
+          <t>"Traumatic Brain Injury" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Acute Care</t>
+          <t>"Traumatic Brain Injury" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>Traumatic Brain Injury Emergency Care</t>
+          <t>"Traumatic Brain Injury" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Trauma neuroinflammation </t>
+          <t>"Brain Trauma" "neuroinflammation "</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Trauma traumatic brain injury </t>
+          <t>"Brain Trauma" "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>Brain Trauma Brain Damage</t>
+          <t>"Brain Trauma" "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Trauma rehabilitation </t>
+          <t>"Brain Trauma" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>Brain Trauma Rehab</t>
+          <t>"Brain Trauma" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>Brain Trauma Therapy</t>
+          <t>"Brain Trauma" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>Brain Trauma Restoration</t>
+          <t>"Brain Trauma" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>Brain Trauma Recovery Program</t>
+          <t>"Brain Trauma" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Trauma Intensive care </t>
+          <t>"Brain Trauma" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>Brain Trauma Critical Care</t>
+          <t>"Brain Trauma" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>Brain Trauma Acute Care</t>
+          <t>"Brain Trauma" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>Brain Trauma Emergency Care</t>
+          <t>"Brain Trauma" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuroinflammation  traumatic brain injury </t>
+          <t>"neuroinflammation " "traumatic brain injury "</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>neuroinflammation  Brain Damage</t>
+          <t>"neuroinflammation " "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuroinflammation  rehabilitation </t>
+          <t>"neuroinflammation " "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>neuroinflammation  Rehab</t>
+          <t>"neuroinflammation " "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>neuroinflammation  Therapy</t>
+          <t>"neuroinflammation " "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>neuroinflammation  Restoration</t>
+          <t>"neuroinflammation " "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>neuroinflammation  Recovery Program</t>
+          <t>"neuroinflammation " "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t xml:space="preserve">neuroinflammation  Intensive care </t>
+          <t>"neuroinflammation " "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>neuroinflammation  Critical Care</t>
+          <t>"neuroinflammation " "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>neuroinflammation  Acute Care</t>
+          <t>"neuroinflammation " "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>neuroinflammation  Emergency Care</t>
+          <t>"neuroinflammation " "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Brain Damage</t>
+          <t>"traumatic brain injury " "Brain Damage"</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t xml:space="preserve">traumatic brain injury  rehabilitation </t>
+          <t>"traumatic brain injury " "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Rehab</t>
+          <t>"traumatic brain injury " "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Therapy</t>
+          <t>"traumatic brain injury " "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Restoration</t>
+          <t>"traumatic brain injury " "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Recovery Program</t>
+          <t>"traumatic brain injury " "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t xml:space="preserve">traumatic brain injury  Intensive care </t>
+          <t>"traumatic brain injury " "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Critical Care</t>
+          <t>"traumatic brain injury " "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Acute Care</t>
+          <t>"traumatic brain injury " "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>traumatic brain injury  Emergency Care</t>
+          <t>"traumatic brain injury " "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Damage rehabilitation </t>
+          <t>"Brain Damage" "rehabilitation "</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>Brain Damage Rehab</t>
+          <t>"Brain Damage" "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>Brain Damage Therapy</t>
+          <t>"Brain Damage" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>Brain Damage Restoration</t>
+          <t>"Brain Damage" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>Brain Damage Recovery Program</t>
+          <t>"Brain Damage" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brain Damage Intensive care </t>
+          <t>"Brain Damage" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>Brain Damage Critical Care</t>
+          <t>"Brain Damage" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>Brain Damage Acute Care</t>
+          <t>"Brain Damage" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>Brain Damage Emergency Care</t>
+          <t>"Brain Damage" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>rehabilitation  Rehab</t>
+          <t>"rehabilitation " "Rehab"</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>rehabilitation  Therapy</t>
+          <t>"rehabilitation " "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>rehabilitation  Restoration</t>
+          <t>"rehabilitation " "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>rehabilitation  Recovery Program</t>
+          <t>"rehabilitation " "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t xml:space="preserve">rehabilitation  Intensive care </t>
+          <t>"rehabilitation " "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>rehabilitation  Critical Care</t>
+          <t>"rehabilitation " "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>rehabilitation  Acute Care</t>
+          <t>"rehabilitation " "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>rehabilitation  Emergency Care</t>
+          <t>"rehabilitation " "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>Rehab Therapy</t>
+          <t>"Rehab" "Therapy"</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>Rehab Restoration</t>
+          <t>"Rehab" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>Rehab Recovery Program</t>
+          <t>"Rehab" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rehab Intensive care </t>
+          <t>"Rehab" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>Rehab Critical Care</t>
+          <t>"Rehab" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>Rehab Acute Care</t>
+          <t>"Rehab" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>Rehab Emergency Care</t>
+          <t>"Rehab" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>Therapy Restoration</t>
+          <t>"Therapy" "Restoration"</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>Therapy Recovery Program</t>
+          <t>"Therapy" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t xml:space="preserve">Therapy Intensive care </t>
+          <t>"Therapy" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>Therapy Critical Care</t>
+          <t>"Therapy" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>Therapy Acute Care</t>
+          <t>"Therapy" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>Therapy Emergency Care</t>
+          <t>"Therapy" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>Restoration Recovery Program</t>
+          <t>"Restoration" "Recovery Program"</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t xml:space="preserve">Restoration Intensive care </t>
+          <t>"Restoration" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>Restoration Critical Care</t>
+          <t>"Restoration" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>Restoration Acute Care</t>
+          <t>"Restoration" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>Restoration Emergency Care</t>
+          <t>"Restoration" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t xml:space="preserve">Recovery Program Intensive care </t>
+          <t>"Recovery Program" "Intensive care "</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>Recovery Program Critical Care</t>
+          <t>"Recovery Program" "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>Recovery Program Acute Care</t>
+          <t>"Recovery Program" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>Recovery Program Emergency Care</t>
+          <t>"Recovery Program" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>Intensive care  Critical Care</t>
+          <t>"Intensive care " "Critical Care"</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>Intensive care  Acute Care</t>
+          <t>"Intensive care " "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>Intensive care  Emergency Care</t>
+          <t>"Intensive care " "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>Critical Care Acute Care</t>
+          <t>"Critical Care" "Acute Care"</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>Critical Care Emergency Care</t>
+          <t>"Critical Care" "Emergency Care"</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>Acute Care Emergency Care</t>
+          <t>"Acute Care" "Emergency Care"</t>
         </is>
       </c>
     </row>

</xml_diff>